<commit_message>
Minor changes in shading nets and plotting fuctions
</commit_message>
<xml_diff>
--- a/CVX_Kenya/Interventions/Pulping_machines.xlsx
+++ b/CVX_Kenya/Interventions/Pulping_machines.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gollinucci\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\Interventions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79CE8FF-922B-44B7-BA1C-E6F7A6416A9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8EC333-3DC0-4E8A-B59E-01419E171AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5625" yWindow="-7875" windowWidth="13830" windowHeight="7170" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -1071,21 +1071,6 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1100,6 +1085,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1694,7 +1694,7 @@
       <c r="F4" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="42">
         <f>main!C33</f>
         <v>0.03</v>
       </c>
@@ -1857,7 +1857,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2541,7 +2541,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2579,7 +2579,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="50" t="s">
         <v>172</v>
       </c>
       <c r="B2" s="17" t="s">
@@ -2593,12 +2593,12 @@
         <v>187</v>
       </c>
       <c r="F2" s="18"/>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="41" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
+      <c r="A3" s="51"/>
       <c r="B3" s="17" t="s">
         <v>173</v>
       </c>
@@ -2613,7 +2613,7 @@
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
+      <c r="A4" s="51"/>
       <c r="B4" s="17" t="s">
         <v>242</v>
       </c>
@@ -2628,7 +2628,7 @@
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
+      <c r="A5" s="51"/>
       <c r="B5" s="17" t="s">
         <v>189</v>
       </c>
@@ -2643,11 +2643,11 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
-      <c r="B6" s="44" t="s">
+      <c r="A6" s="51"/>
+      <c r="B6" s="39" t="s">
         <v>236</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="40">
         <v>0</v>
       </c>
       <c r="D6" s="24"/>
@@ -2655,12 +2655,12 @@
         <v>237</v>
       </c>
       <c r="F6" s="18"/>
-      <c r="G6" s="46" t="s">
+      <c r="G6" s="41" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
+      <c r="A7" s="51"/>
       <c r="B7" s="17" t="s">
         <v>191</v>
       </c>
@@ -2673,7 +2673,7 @@
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
+      <c r="A8" s="51"/>
       <c r="B8" s="17" t="s">
         <v>194</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="41"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="17" t="s">
         <v>198</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="51"/>
       <c r="B10" s="17" t="s">
         <v>201</v>
       </c>
@@ -2716,7 +2716,7 @@
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
+      <c r="A11" s="51"/>
       <c r="B11" s="17" t="s">
         <v>200</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="G11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="17" t="s">
         <v>207</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="41"/>
+      <c r="A13" s="51"/>
       <c r="B13" s="17" t="s">
         <v>209</v>
       </c>
@@ -2761,7 +2761,7 @@
       <c r="G13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="41"/>
+      <c r="A14" s="51"/>
       <c r="B14" s="17" t="s">
         <v>210</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="G14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
+      <c r="A15" s="51"/>
       <c r="B15" s="17" t="s">
         <v>186</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="G15" s="18"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
+      <c r="A16" s="51"/>
       <c r="B16" s="17" t="s">
         <v>228</v>
       </c>
@@ -2806,22 +2806,22 @@
       <c r="G16" s="18"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="48" t="s">
+      <c r="A17" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="C17" s="50">
+      <c r="C17" s="45">
         <v>6</v>
       </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="A18" s="49" t="s">
         <v>180</v>
       </c>
       <c r="B18" s="16" t="s">
@@ -2836,7 +2836,7 @@
       <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="16" t="s">
         <v>188</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="G19" s="21"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="16" t="s">
         <v>225</v>
       </c>
@@ -2864,7 +2864,7 @@
       <c r="G20" s="21"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="42" t="s">
+      <c r="A21" s="48" t="s">
         <v>181</v>
       </c>
       <c r="B21" s="22" t="s">
@@ -2882,7 +2882,7 @@
       <c r="G21" s="23"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="42"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="29" t="s">
         <v>226</v>
       </c>
@@ -2896,7 +2896,7 @@
       <c r="G22" s="23"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="42"/>
+      <c r="A23" s="48"/>
       <c r="B23" s="29" t="s">
         <v>185</v>
       </c>
@@ -2910,7 +2910,7 @@
       <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
+      <c r="A24" s="48"/>
       <c r="B24" s="22" t="s">
         <v>204</v>
       </c>
@@ -2926,7 +2926,7 @@
       <c r="G24" s="23"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="42"/>
+      <c r="A25" s="48"/>
       <c r="B25" s="22" t="s">
         <v>235</v>
       </c>
@@ -2942,7 +2942,7 @@
       <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="42"/>
+      <c r="A26" s="48"/>
       <c r="B26" s="22" t="s">
         <v>206</v>
       </c>
@@ -2958,7 +2958,7 @@
       <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="47" t="s">
         <v>182</v>
       </c>
       <c r="B27" s="19" t="s">
@@ -2978,7 +2978,7 @@
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="39"/>
+      <c r="A28" s="47"/>
       <c r="B28" s="19" t="s">
         <v>184</v>
       </c>
@@ -2996,7 +2996,7 @@
       <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="39"/>
+      <c r="A29" s="47"/>
       <c r="B29" s="19" t="s">
         <v>185</v>
       </c>
@@ -3014,7 +3014,7 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="39"/>
+      <c r="A30" s="47"/>
       <c r="B30" s="19" t="s">
         <v>192</v>
       </c>
@@ -3032,7 +3032,7 @@
       <c r="G30" s="20"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="39"/>
+      <c r="A31" s="47"/>
       <c r="B31" s="19" t="s">
         <v>234</v>
       </c>
@@ -3050,7 +3050,7 @@
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="39"/>
+      <c r="A32" s="47"/>
       <c r="B32" s="19" t="s">
         <v>230</v>
       </c>
@@ -3068,7 +3068,7 @@
       <c r="G32" s="20"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="39"/>
+      <c r="A33" s="47"/>
       <c r="B33" s="19" t="s">
         <v>243</v>
       </c>
@@ -3086,7 +3086,7 @@
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="39"/>
+      <c r="A34" s="47"/>
       <c r="B34" s="19" t="s">
         <v>193</v>
       </c>

</xml_diff>